<commit_message>
#249: added test case and updated test file
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/NvPr.xlsx
+++ b/EPPlusTest/Workbooks/NvPr.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="21570" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="21570" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>picture:</t>
   </si>
@@ -33,6 +33,18 @@
   </si>
   <si>
     <t>chart:</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
   </si>
 </sst>
 </file>
@@ -158,11 +170,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="126805624"/>
-        <c:axId val="420726896"/>
+        <c:axId val="221663656"/>
+        <c:axId val="221667184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126805624"/>
+        <c:axId val="221663656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -203,7 +215,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420726896"/>
+        <c:crossAx val="221667184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -211,7 +223,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="420726896"/>
+        <c:axId val="221667184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -260,7 +272,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126805624"/>
+        <c:crossAx val="221663656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -984,6 +996,19 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" comment="Luke, I am your father... seriously..." ref="O4:R13" totalsRowShown="0">
+  <autoFilter ref="O4:R13"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1249,15 +1274,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:M4"/>
+  <dimension ref="A4:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="18" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1277,6 +1305,18 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1286,5 +1326,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>